<commit_message>
Created a toolbox module for methods
</commit_message>
<xml_diff>
--- a/Interface Excel.xlsx
+++ b/Interface Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Documents\Dauphine Offline\Projet C#\Projet_C_sharp_Pricer_Structured_Poduct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BF6C14-09AB-48CC-AB27-C0B102E97B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC99DC00-A695-434E-90C0-ABE6D7EC7EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{E403B6F2-3256-482E-B553-E70ADB64458A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E403B6F2-3256-482E-B553-E70ADB64458A}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="637">
   <si>
     <t>Notionnel</t>
   </si>
@@ -1950,6 +1950,15 @@
   </si>
   <si>
     <t>Funding</t>
+  </si>
+  <si>
+    <t>Reoffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limiter au produit dans la liste on retire les matu </t>
+  </si>
+  <si>
+    <t>on solve pour coupon, matu, reoffer</t>
   </si>
 </sst>
 </file>
@@ -2447,7 +2456,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2483,7 +2492,6 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2548,7 +2556,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2889,7 +2900,7 @@
   <dimension ref="B4:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2899,11 +2910,12 @@
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2912,128 +2924,152 @@
       <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>10000000</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
       <c r="J5" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="E6" s="30" t="s">
+      <c r="C6" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>602</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="37">
-        <v>49096</v>
-      </c>
-      <c r="E7" s="31" t="s">
+      <c r="C7" s="36">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="28" t="str">
+      <c r="F7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="27">
         <f>IF(F7="","",VLOOKUP(F7,Univers!$B$2:$D$357,2,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H7" s="32" t="str">
+        <v>0</v>
+      </c>
+      <c r="H7" s="31" t="str">
         <f>IF(F7="","",VLOOKUP(F7,Univers!$B$2:$D$357,3,FALSE))</f>
-        <v/>
-      </c>
-      <c r="J7" s="54" t="s">
+        <v>FR001400J770</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="E8" s="31" t="s">
+      <c r="C8" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="28" t="str">
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="27" t="str">
         <f>IF(F8="","",VLOOKUP(F8,Univers!$B$2:$D$357,2,FALSE))</f>
-        <v/>
-      </c>
-      <c r="H8" s="32" t="str">
+        <v>AC FP Equity</v>
+      </c>
+      <c r="H8" s="31">
         <f>IF(F8="","",VLOOKUP(F8,Univers!$B$2:$D$357,3,FALSE))</f>
-        <v/>
-      </c>
-      <c r="J8" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="E9" s="31" t="s">
+      <c r="C9" s="37"/>
+      <c r="E9" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="28" t="str">
+      <c r="G9" s="27" t="str">
         <f>IF(F9="","",VLOOKUP(F9,Univers!$B$2:$D$357,2,FALSE))</f>
         <v/>
       </c>
-      <c r="H9" s="32" t="str">
+      <c r="H9" s="31" t="str">
         <f>IF(F9="","",VLOOKUP(F9,Univers!$B$2:$D$357,3,FALSE))</f>
         <v/>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="E10" s="33" t="s">
+      <c r="C10" s="56"/>
+      <c r="E10" s="32" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="34" t="str">
+      <c r="G10" s="33" t="str">
         <f>IF(F10="","",VLOOKUP(F10,Univers!$B$2:$D$357,2,FALSE))</f>
         <v/>
       </c>
-      <c r="H10" s="35" t="str">
+      <c r="H10" s="34" t="str">
         <f>IF(F10="","",VLOOKUP(F10,Univers!$B$2:$D$357,3,FALSE))</f>
         <v/>
       </c>
-      <c r="J10" s="54" t="s">
+      <c r="J10" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="53" t="s">
+        <v>634</v>
+      </c>
+      <c r="C11" s="54"/>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H19" s="24"/>
+      <c r="K19" s="1" t="s">
+        <v>636</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -3191,7 +3227,7 @@
   <dimension ref="A1:F241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,22 +3242,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>603</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>604</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>605</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>570</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>571</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>609</v>
       </c>
     </row>
@@ -4508,8 +4544,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D357"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="B357" sqref="B357"/>
+    <sheetView showGridLines="0" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4536,7 +4572,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>562</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -4548,7 +4584,7 @@
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="46"/>
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -4558,7 +4594,7 @@
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
@@ -4568,7 +4604,7 @@
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="16" t="s">
         <v>14</v>
       </c>
@@ -4578,7 +4614,7 @@
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
@@ -4588,7 +4624,7 @@
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
@@ -4598,7 +4634,7 @@
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
       </c>
@@ -4608,7 +4644,7 @@
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="16" t="s">
         <v>18</v>
       </c>
@@ -4618,7 +4654,7 @@
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="16" t="s">
         <v>19</v>
       </c>
@@ -4628,7 +4664,7 @@
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="16" t="s">
         <v>20</v>
       </c>
@@ -4638,7 +4674,7 @@
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="16" t="s">
         <v>21</v>
       </c>
@@ -4648,7 +4684,7 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="16" t="s">
         <v>22</v>
       </c>
@@ -4658,7 +4694,7 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="16" t="s">
         <v>23</v>
       </c>
@@ -4668,7 +4704,7 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="16" t="s">
         <v>24</v>
       </c>
@@ -4678,7 +4714,7 @@
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="16" t="s">
         <v>25</v>
       </c>
@@ -4688,7 +4724,7 @@
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="16" t="s">
         <v>26</v>
       </c>
@@ -4698,7 +4734,7 @@
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="16" t="s">
         <v>27</v>
       </c>
@@ -4708,7 +4744,7 @@
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="16" t="s">
         <v>28</v>
       </c>
@@ -4718,7 +4754,7 @@
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="16" t="s">
         <v>29</v>
       </c>
@@ -4728,7 +4764,7 @@
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="16" t="s">
         <v>30</v>
       </c>
@@ -4738,7 +4774,7 @@
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="16" t="s">
         <v>31</v>
       </c>
@@ -4748,7 +4784,7 @@
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="16" t="s">
         <v>32</v>
       </c>
@@ -4758,7 +4794,7 @@
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="16" t="s">
         <v>33</v>
       </c>
@@ -4768,7 +4804,7 @@
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="16" t="s">
         <v>34</v>
       </c>
@@ -4778,7 +4814,7 @@
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="16" t="s">
         <v>35</v>
       </c>
@@ -4788,7 +4824,7 @@
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="16" t="s">
         <v>36</v>
       </c>
@@ -4798,7 +4834,7 @@
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="16" t="s">
         <v>37</v>
       </c>
@@ -4808,7 +4844,7 @@
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="16" t="s">
         <v>38</v>
       </c>
@@ -4818,7 +4854,7 @@
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="16" t="s">
         <v>39</v>
       </c>
@@ -4828,7 +4864,7 @@
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="16" t="s">
         <v>40</v>
       </c>
@@ -4838,7 +4874,7 @@
       <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="16" t="s">
         <v>41</v>
       </c>
@@ -4848,7 +4884,7 @@
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="16" t="s">
         <v>42</v>
       </c>
@@ -4858,7 +4894,7 @@
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="46"/>
       <c r="B34" s="16" t="s">
         <v>43</v>
       </c>
@@ -4868,7 +4904,7 @@
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="16" t="s">
         <v>44</v>
       </c>
@@ -4878,7 +4914,7 @@
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="46"/>
       <c r="B36" s="16" t="s">
         <v>45</v>
       </c>
@@ -4888,7 +4924,7 @@
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="16" t="s">
         <v>46</v>
       </c>
@@ -4898,7 +4934,7 @@
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="16" t="s">
         <v>47</v>
       </c>
@@ -4908,7 +4944,7 @@
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="16" t="s">
         <v>48</v>
       </c>
@@ -4918,7 +4954,7 @@
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="16" t="s">
         <v>49</v>
       </c>
@@ -4928,7 +4964,7 @@
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="48"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="16" t="s">
         <v>50</v>
       </c>
@@ -4938,7 +4974,7 @@
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="45" t="s">
         <v>176</v>
       </c>
       <c r="B42" s="16" t="s">
@@ -4950,7 +4986,7 @@
       <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="16" t="s">
         <v>98</v>
       </c>
@@ -4960,7 +4996,7 @@
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="16" t="s">
         <v>99</v>
       </c>
@@ -4970,7 +5006,7 @@
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="46"/>
       <c r="B45" s="16" t="s">
         <v>100</v>
       </c>
@@ -4980,7 +5016,7 @@
       <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="46"/>
       <c r="B46" s="16" t="s">
         <v>101</v>
       </c>
@@ -4990,7 +5026,7 @@
       <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
+      <c r="A47" s="46"/>
       <c r="B47" s="16" t="s">
         <v>102</v>
       </c>
@@ -5000,7 +5036,7 @@
       <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="A48" s="46"/>
       <c r="B48" s="16" t="s">
         <v>96</v>
       </c>
@@ -5010,7 +5046,7 @@
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
+      <c r="A49" s="46"/>
       <c r="B49" s="16" t="s">
         <v>103</v>
       </c>
@@ -5020,7 +5056,7 @@
       <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
+      <c r="A50" s="46"/>
       <c r="B50" s="16" t="s">
         <v>104</v>
       </c>
@@ -5030,7 +5066,7 @@
       <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
+      <c r="A51" s="46"/>
       <c r="B51" s="16" t="s">
         <v>105</v>
       </c>
@@ -5040,7 +5076,7 @@
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
+      <c r="A52" s="46"/>
       <c r="B52" s="16" t="s">
         <v>106</v>
       </c>
@@ -5050,7 +5086,7 @@
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
+      <c r="A53" s="46"/>
       <c r="B53" s="16" t="s">
         <v>93</v>
       </c>
@@ -5060,7 +5096,7 @@
       <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
+      <c r="A54" s="46"/>
       <c r="B54" s="16" t="s">
         <v>107</v>
       </c>
@@ -5070,7 +5106,7 @@
       <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="16" t="s">
         <v>108</v>
       </c>
@@ -5080,7 +5116,7 @@
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
+      <c r="A56" s="46"/>
       <c r="B56" s="16" t="s">
         <v>109</v>
       </c>
@@ -5090,7 +5126,7 @@
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
+      <c r="A57" s="46"/>
       <c r="B57" s="16" t="s">
         <v>110</v>
       </c>
@@ -5100,7 +5136,7 @@
       <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="47"/>
+      <c r="A58" s="46"/>
       <c r="B58" s="16" t="s">
         <v>111</v>
       </c>
@@ -5110,7 +5146,7 @@
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="47"/>
+      <c r="A59" s="46"/>
       <c r="B59" s="16" t="s">
         <v>112</v>
       </c>
@@ -5120,7 +5156,7 @@
       <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
+      <c r="A60" s="46"/>
       <c r="B60" s="16" t="s">
         <v>95</v>
       </c>
@@ -5130,7 +5166,7 @@
       <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
+      <c r="A61" s="46"/>
       <c r="B61" s="16" t="s">
         <v>94</v>
       </c>
@@ -5140,7 +5176,7 @@
       <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
+      <c r="A62" s="46"/>
       <c r="B62" s="16" t="s">
         <v>113</v>
       </c>
@@ -5150,7 +5186,7 @@
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
+      <c r="A63" s="46"/>
       <c r="B63" s="16" t="s">
         <v>114</v>
       </c>
@@ -5160,7 +5196,7 @@
       <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
+      <c r="A64" s="46"/>
       <c r="B64" s="16" t="s">
         <v>115</v>
       </c>
@@ -5170,7 +5206,7 @@
       <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="47"/>
+      <c r="A65" s="46"/>
       <c r="B65" s="16" t="s">
         <v>116</v>
       </c>
@@ -5180,7 +5216,7 @@
       <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="47"/>
+      <c r="A66" s="46"/>
       <c r="B66" s="16" t="s">
         <v>117</v>
       </c>
@@ -5190,7 +5226,7 @@
       <c r="D66" s="7"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="47"/>
+      <c r="A67" s="46"/>
       <c r="B67" s="16" t="s">
         <v>118</v>
       </c>
@@ -5200,7 +5236,7 @@
       <c r="D67" s="7"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
+      <c r="A68" s="46"/>
       <c r="B68" s="16" t="s">
         <v>119</v>
       </c>
@@ -5210,7 +5246,7 @@
       <c r="D68" s="7"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="47"/>
+      <c r="A69" s="46"/>
       <c r="B69" s="16" t="s">
         <v>120</v>
       </c>
@@ -5220,7 +5256,7 @@
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
+      <c r="A70" s="46"/>
       <c r="B70" s="16" t="s">
         <v>121</v>
       </c>
@@ -5230,7 +5266,7 @@
       <c r="D70" s="7"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="47"/>
+      <c r="A71" s="46"/>
       <c r="B71" s="16" t="s">
         <v>122</v>
       </c>
@@ -5240,7 +5276,7 @@
       <c r="D71" s="7"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="47"/>
+      <c r="A72" s="46"/>
       <c r="B72" s="16" t="s">
         <v>123</v>
       </c>
@@ -5250,7 +5286,7 @@
       <c r="D72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="47"/>
+      <c r="A73" s="46"/>
       <c r="B73" s="16" t="s">
         <v>124</v>
       </c>
@@ -5260,7 +5296,7 @@
       <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
+      <c r="A74" s="46"/>
       <c r="B74" s="16" t="s">
         <v>125</v>
       </c>
@@ -5270,7 +5306,7 @@
       <c r="D74" s="7"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="47"/>
+      <c r="A75" s="46"/>
       <c r="B75" s="16" t="s">
         <v>126</v>
       </c>
@@ -5280,7 +5316,7 @@
       <c r="D75" s="7"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="47"/>
+      <c r="A76" s="46"/>
       <c r="B76" s="16" t="s">
         <v>127</v>
       </c>
@@ -5290,7 +5326,7 @@
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="47"/>
+      <c r="A77" s="46"/>
       <c r="B77" s="16" t="s">
         <v>128</v>
       </c>
@@ -5300,7 +5336,7 @@
       <c r="D77" s="7"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="47"/>
+      <c r="A78" s="46"/>
       <c r="B78" s="16" t="s">
         <v>129</v>
       </c>
@@ -5310,7 +5346,7 @@
       <c r="D78" s="7"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
+      <c r="A79" s="46"/>
       <c r="B79" s="16" t="s">
         <v>130</v>
       </c>
@@ -5320,7 +5356,7 @@
       <c r="D79" s="7"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
+      <c r="A80" s="46"/>
       <c r="B80" s="16" t="s">
         <v>131</v>
       </c>
@@ -5330,7 +5366,7 @@
       <c r="D80" s="7"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
+      <c r="A81" s="46"/>
       <c r="B81" s="16" t="s">
         <v>132</v>
       </c>
@@ -5340,7 +5376,7 @@
       <c r="D81" s="7"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="47"/>
+      <c r="A82" s="46"/>
       <c r="B82" s="16" t="s">
         <v>133</v>
       </c>
@@ -5350,7 +5386,7 @@
       <c r="D82" s="7"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="47"/>
+      <c r="A83" s="46"/>
       <c r="B83" s="16" t="s">
         <v>134</v>
       </c>
@@ -5360,7 +5396,7 @@
       <c r="D83" s="7"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
+      <c r="A84" s="46"/>
       <c r="B84" s="16" t="s">
         <v>135</v>
       </c>
@@ -5370,7 +5406,7 @@
       <c r="D84" s="7"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="47"/>
+      <c r="A85" s="46"/>
       <c r="B85" s="16" t="s">
         <v>136</v>
       </c>
@@ -5380,7 +5416,7 @@
       <c r="D85" s="7"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="47"/>
+      <c r="A86" s="46"/>
       <c r="B86" s="16" t="s">
         <v>137</v>
       </c>
@@ -5390,7 +5426,7 @@
       <c r="D86" s="7"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="47"/>
+      <c r="A87" s="46"/>
       <c r="B87" s="16" t="s">
         <v>138</v>
       </c>
@@ -5400,7 +5436,7 @@
       <c r="D87" s="7"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="47"/>
+      <c r="A88" s="46"/>
       <c r="B88" s="16" t="s">
         <v>139</v>
       </c>
@@ -5410,7 +5446,7 @@
       <c r="D88" s="7"/>
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="48"/>
+      <c r="A89" s="47"/>
       <c r="B89" s="16" t="s">
         <v>140</v>
       </c>
@@ -5420,7 +5456,7 @@
       <c r="D89" s="7"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="46" t="s">
+      <c r="A90" s="45" t="s">
         <v>563</v>
       </c>
       <c r="B90" s="16" t="s">
@@ -5432,7 +5468,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="47"/>
+      <c r="A91" s="46"/>
       <c r="B91" s="16" t="s">
         <v>180</v>
       </c>
@@ -5442,7 +5478,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="47"/>
+      <c r="A92" s="46"/>
       <c r="B92" s="16" t="s">
         <v>182</v>
       </c>
@@ -5452,7 +5488,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="47"/>
+      <c r="A93" s="46"/>
       <c r="B93" s="16" t="s">
         <v>12</v>
       </c>
@@ -5462,7 +5498,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="47"/>
+      <c r="A94" s="46"/>
       <c r="B94" s="16" t="s">
         <v>185</v>
       </c>
@@ -5472,7 +5508,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="47"/>
+      <c r="A95" s="46"/>
       <c r="B95" s="16" t="s">
         <v>188</v>
       </c>
@@ -5482,7 +5518,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="47"/>
+      <c r="A96" s="46"/>
       <c r="B96" s="16" t="s">
         <v>190</v>
       </c>
@@ -5492,7 +5528,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="47"/>
+      <c r="A97" s="46"/>
       <c r="B97" s="16" t="s">
         <v>192</v>
       </c>
@@ -5502,7 +5538,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="47"/>
+      <c r="A98" s="46"/>
       <c r="B98" s="16" t="s">
         <v>194</v>
       </c>
@@ -5512,7 +5548,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="47"/>
+      <c r="A99" s="46"/>
       <c r="B99" s="16" t="s">
         <v>196</v>
       </c>
@@ -5522,7 +5558,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="47"/>
+      <c r="A100" s="46"/>
       <c r="B100" s="16" t="s">
         <v>200</v>
       </c>
@@ -5532,7 +5568,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="47"/>
+      <c r="A101" s="46"/>
       <c r="B101" s="16" t="s">
         <v>202</v>
       </c>
@@ -5542,7 +5578,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="47"/>
+      <c r="A102" s="46"/>
       <c r="B102" s="16" t="s">
         <v>204</v>
       </c>
@@ -5552,7 +5588,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="47"/>
+      <c r="A103" s="46"/>
       <c r="B103" s="16" t="s">
         <v>206</v>
       </c>
@@ -5562,7 +5598,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="47"/>
+      <c r="A104" s="46"/>
       <c r="B104" s="16" t="s">
         <v>15</v>
       </c>
@@ -5572,7 +5608,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="47"/>
+      <c r="A105" s="46"/>
       <c r="B105" s="16" t="s">
         <v>209</v>
       </c>
@@ -5582,7 +5618,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="47"/>
+      <c r="A106" s="46"/>
       <c r="B106" s="16" t="s">
         <v>211</v>
       </c>
@@ -5592,7 +5628,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="47"/>
+      <c r="A107" s="46"/>
       <c r="B107" s="16" t="s">
         <v>213</v>
       </c>
@@ -5602,7 +5638,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="47"/>
+      <c r="A108" s="46"/>
       <c r="B108" s="16" t="s">
         <v>215</v>
       </c>
@@ -5612,7 +5648,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="47"/>
+      <c r="A109" s="46"/>
       <c r="B109" s="16" t="s">
         <v>217</v>
       </c>
@@ -5622,7 +5658,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="47"/>
+      <c r="A110" s="46"/>
       <c r="B110" s="16" t="s">
         <v>17</v>
       </c>
@@ -5632,7 +5668,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="47"/>
+      <c r="A111" s="46"/>
       <c r="B111" s="16" t="s">
         <v>220</v>
       </c>
@@ -5642,7 +5678,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="47"/>
+      <c r="A112" s="46"/>
       <c r="B112" s="16" t="s">
         <v>18</v>
       </c>
@@ -5652,7 +5688,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="47"/>
+      <c r="A113" s="46"/>
       <c r="B113" s="16" t="s">
         <v>223</v>
       </c>
@@ -5662,7 +5698,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="47"/>
+      <c r="A114" s="46"/>
       <c r="B114" s="16" t="s">
         <v>19</v>
       </c>
@@ -5672,7 +5708,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="47"/>
+      <c r="A115" s="46"/>
       <c r="B115" s="16" t="s">
         <v>226</v>
       </c>
@@ -5682,7 +5718,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="47"/>
+      <c r="A116" s="46"/>
       <c r="B116" s="16" t="s">
         <v>228</v>
       </c>
@@ -5692,7 +5728,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="47"/>
+      <c r="A117" s="46"/>
       <c r="B117" s="16" t="s">
         <v>230</v>
       </c>
@@ -5702,7 +5738,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="47"/>
+      <c r="A118" s="46"/>
       <c r="B118" s="16" t="s">
         <v>20</v>
       </c>
@@ -5712,7 +5748,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="47"/>
+      <c r="A119" s="46"/>
       <c r="B119" s="16" t="s">
         <v>21</v>
       </c>
@@ -5722,7 +5758,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="47"/>
+      <c r="A120" s="46"/>
       <c r="B120" s="16" t="s">
         <v>234</v>
       </c>
@@ -5732,7 +5768,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="47"/>
+      <c r="A121" s="46"/>
       <c r="B121" s="16" t="s">
         <v>22</v>
       </c>
@@ -5742,7 +5778,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="47"/>
+      <c r="A122" s="46"/>
       <c r="B122" s="16" t="s">
         <v>237</v>
       </c>
@@ -5752,7 +5788,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="47"/>
+      <c r="A123" s="46"/>
       <c r="B123" s="16" t="s">
         <v>23</v>
       </c>
@@ -5762,7 +5798,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="47"/>
+      <c r="A124" s="46"/>
       <c r="B124" s="16" t="s">
         <v>240</v>
       </c>
@@ -5772,7 +5808,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="47"/>
+      <c r="A125" s="46"/>
       <c r="B125" s="16" t="s">
         <v>242</v>
       </c>
@@ -5782,7 +5818,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="47"/>
+      <c r="A126" s="46"/>
       <c r="B126" s="16" t="s">
         <v>244</v>
       </c>
@@ -5792,7 +5828,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="47"/>
+      <c r="A127" s="46"/>
       <c r="B127" s="16" t="s">
         <v>24</v>
       </c>
@@ -5802,7 +5838,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="47"/>
+      <c r="A128" s="46"/>
       <c r="B128" s="16" t="s">
         <v>247</v>
       </c>
@@ -5812,7 +5848,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="47"/>
+      <c r="A129" s="46"/>
       <c r="B129" s="16" t="s">
         <v>25</v>
       </c>
@@ -5822,7 +5858,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="47"/>
+      <c r="A130" s="46"/>
       <c r="B130" s="16" t="s">
         <v>250</v>
       </c>
@@ -5832,7 +5868,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="47"/>
+      <c r="A131" s="46"/>
       <c r="B131" s="16" t="s">
         <v>252</v>
       </c>
@@ -5842,7 +5878,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="47"/>
+      <c r="A132" s="46"/>
       <c r="B132" s="16" t="s">
         <v>254</v>
       </c>
@@ -5852,7 +5888,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="47"/>
+      <c r="A133" s="46"/>
       <c r="B133" s="16" t="s">
         <v>256</v>
       </c>
@@ -5862,7 +5898,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="47"/>
+      <c r="A134" s="46"/>
       <c r="B134" s="16" t="s">
         <v>258</v>
       </c>
@@ -5872,7 +5908,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="47"/>
+      <c r="A135" s="46"/>
       <c r="B135" s="16" t="s">
         <v>260</v>
       </c>
@@ -5882,7 +5918,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="47"/>
+      <c r="A136" s="46"/>
       <c r="B136" s="16" t="s">
         <v>262</v>
       </c>
@@ -5892,7 +5928,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="47"/>
+      <c r="A137" s="46"/>
       <c r="B137" s="16" t="s">
         <v>264</v>
       </c>
@@ -5902,7 +5938,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="47"/>
+      <c r="A138" s="46"/>
       <c r="B138" s="16" t="s">
         <v>266</v>
       </c>
@@ -5912,7 +5948,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="47"/>
+      <c r="A139" s="46"/>
       <c r="B139" s="16" t="s">
         <v>268</v>
       </c>
@@ -5922,7 +5958,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="47"/>
+      <c r="A140" s="46"/>
       <c r="B140" s="16" t="s">
         <v>27</v>
       </c>
@@ -5932,7 +5968,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="47"/>
+      <c r="A141" s="46"/>
       <c r="B141" s="16" t="s">
         <v>271</v>
       </c>
@@ -5942,7 +5978,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="47"/>
+      <c r="A142" s="46"/>
       <c r="B142" s="16" t="s">
         <v>273</v>
       </c>
@@ -5952,7 +5988,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="47"/>
+      <c r="A143" s="46"/>
       <c r="B143" s="16" t="s">
         <v>275</v>
       </c>
@@ -5962,7 +5998,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="47"/>
+      <c r="A144" s="46"/>
       <c r="B144" s="16" t="s">
         <v>277</v>
       </c>
@@ -5972,7 +6008,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="47"/>
+      <c r="A145" s="46"/>
       <c r="B145" s="16" t="s">
         <v>279</v>
       </c>
@@ -5982,7 +6018,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="47"/>
+      <c r="A146" s="46"/>
       <c r="B146" s="16" t="s">
         <v>281</v>
       </c>
@@ -5992,7 +6028,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="47"/>
+      <c r="A147" s="46"/>
       <c r="B147" s="16" t="s">
         <v>283</v>
       </c>
@@ -6002,7 +6038,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="47"/>
+      <c r="A148" s="46"/>
       <c r="B148" s="16" t="s">
         <v>28</v>
       </c>
@@ -6012,7 +6048,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="47"/>
+      <c r="A149" s="46"/>
       <c r="B149" s="16" t="s">
         <v>286</v>
       </c>
@@ -6022,7 +6058,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="47"/>
+      <c r="A150" s="46"/>
       <c r="B150" s="16" t="s">
         <v>29</v>
       </c>
@@ -6032,7 +6068,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="47"/>
+      <c r="A151" s="46"/>
       <c r="B151" s="16" t="s">
         <v>289</v>
       </c>
@@ -6042,7 +6078,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="47"/>
+      <c r="A152" s="46"/>
       <c r="B152" s="16" t="s">
         <v>30</v>
       </c>
@@ -6052,7 +6088,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="47"/>
+      <c r="A153" s="46"/>
       <c r="B153" s="16" t="s">
         <v>31</v>
       </c>
@@ -6062,7 +6098,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="47"/>
+      <c r="A154" s="46"/>
       <c r="B154" s="16" t="s">
         <v>293</v>
       </c>
@@ -6072,7 +6108,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="47"/>
+      <c r="A155" s="46"/>
       <c r="B155" s="16" t="s">
         <v>295</v>
       </c>
@@ -6082,7 +6118,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="47"/>
+      <c r="A156" s="46"/>
       <c r="B156" s="16" t="s">
         <v>297</v>
       </c>
@@ -6092,7 +6128,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="47"/>
+      <c r="A157" s="46"/>
       <c r="B157" s="16" t="s">
         <v>299</v>
       </c>
@@ -6102,7 +6138,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="47"/>
+      <c r="A158" s="46"/>
       <c r="B158" s="16" t="s">
         <v>32</v>
       </c>
@@ -6112,7 +6148,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="47"/>
+      <c r="A159" s="46"/>
       <c r="B159" s="16" t="s">
         <v>302</v>
       </c>
@@ -6122,7 +6158,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="47"/>
+      <c r="A160" s="46"/>
       <c r="B160" s="16" t="s">
         <v>304</v>
       </c>
@@ -6132,7 +6168,7 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="47"/>
+      <c r="A161" s="46"/>
       <c r="B161" s="16" t="s">
         <v>306</v>
       </c>
@@ -6142,7 +6178,7 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="47"/>
+      <c r="A162" s="46"/>
       <c r="B162" s="16" t="s">
         <v>33</v>
       </c>
@@ -6152,7 +6188,7 @@
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="47"/>
+      <c r="A163" s="46"/>
       <c r="B163" s="16" t="s">
         <v>309</v>
       </c>
@@ -6162,7 +6198,7 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="47"/>
+      <c r="A164" s="46"/>
       <c r="B164" s="16" t="s">
         <v>311</v>
       </c>
@@ -6172,7 +6208,7 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="47"/>
+      <c r="A165" s="46"/>
       <c r="B165" s="16" t="s">
         <v>313</v>
       </c>
@@ -6182,7 +6218,7 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="47"/>
+      <c r="A166" s="46"/>
       <c r="B166" s="16" t="s">
         <v>315</v>
       </c>
@@ -6192,7 +6228,7 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="47"/>
+      <c r="A167" s="46"/>
       <c r="B167" s="16" t="s">
         <v>317</v>
       </c>
@@ -6202,7 +6238,7 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="47"/>
+      <c r="A168" s="46"/>
       <c r="B168" s="16" t="s">
         <v>319</v>
       </c>
@@ -6212,7 +6248,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="47"/>
+      <c r="A169" s="46"/>
       <c r="B169" s="16" t="s">
         <v>36</v>
       </c>
@@ -6222,7 +6258,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="47"/>
+      <c r="A170" s="46"/>
       <c r="B170" s="16" t="s">
         <v>322</v>
       </c>
@@ -6232,7 +6268,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="47"/>
+      <c r="A171" s="46"/>
       <c r="B171" s="16" t="s">
         <v>324</v>
       </c>
@@ -6242,7 +6278,7 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="47"/>
+      <c r="A172" s="46"/>
       <c r="B172" s="16" t="s">
         <v>326</v>
       </c>
@@ -6252,7 +6288,7 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="47"/>
+      <c r="A173" s="46"/>
       <c r="B173" s="16" t="s">
         <v>37</v>
       </c>
@@ -6262,7 +6298,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="47"/>
+      <c r="A174" s="46"/>
       <c r="B174" s="16" t="s">
         <v>329</v>
       </c>
@@ -6272,7 +6308,7 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="47"/>
+      <c r="A175" s="46"/>
       <c r="B175" s="16" t="s">
         <v>39</v>
       </c>
@@ -6282,7 +6318,7 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="47"/>
+      <c r="A176" s="46"/>
       <c r="B176" s="16" t="s">
         <v>332</v>
       </c>
@@ -6292,7 +6328,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="47"/>
+      <c r="A177" s="46"/>
       <c r="B177" s="16" t="s">
         <v>40</v>
       </c>
@@ -6302,7 +6338,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="47"/>
+      <c r="A178" s="46"/>
       <c r="B178" s="16" t="s">
         <v>335</v>
       </c>
@@ -6312,7 +6348,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="47"/>
+      <c r="A179" s="46"/>
       <c r="B179" s="16" t="s">
         <v>337</v>
       </c>
@@ -6322,7 +6358,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="47"/>
+      <c r="A180" s="46"/>
       <c r="B180" s="16" t="s">
         <v>41</v>
       </c>
@@ -6332,7 +6368,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="47"/>
+      <c r="A181" s="46"/>
       <c r="B181" s="16" t="s">
         <v>340</v>
       </c>
@@ -6342,7 +6378,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="47"/>
+      <c r="A182" s="46"/>
       <c r="B182" s="16" t="s">
         <v>342</v>
       </c>
@@ -6352,7 +6388,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="47"/>
+      <c r="A183" s="46"/>
       <c r="B183" s="16" t="s">
         <v>344</v>
       </c>
@@ -6362,7 +6398,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="47"/>
+      <c r="A184" s="46"/>
       <c r="B184" s="16" t="s">
         <v>346</v>
       </c>
@@ -6372,7 +6408,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="47"/>
+      <c r="A185" s="46"/>
       <c r="B185" s="16" t="s">
         <v>350</v>
       </c>
@@ -6382,7 +6418,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="47"/>
+      <c r="A186" s="46"/>
       <c r="B186" s="16" t="s">
         <v>352</v>
       </c>
@@ -6392,7 +6428,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="47"/>
+      <c r="A187" s="46"/>
       <c r="B187" s="16" t="s">
         <v>42</v>
       </c>
@@ -6402,7 +6438,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="47"/>
+      <c r="A188" s="46"/>
       <c r="B188" s="16" t="s">
         <v>43</v>
       </c>
@@ -6412,7 +6448,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="47"/>
+      <c r="A189" s="46"/>
       <c r="B189" s="16" t="s">
         <v>356</v>
       </c>
@@ -6422,7 +6458,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="47"/>
+      <c r="A190" s="46"/>
       <c r="B190" s="16" t="s">
         <v>44</v>
       </c>
@@ -6432,7 +6468,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="47"/>
+      <c r="A191" s="46"/>
       <c r="B191" s="16" t="s">
         <v>359</v>
       </c>
@@ -6442,7 +6478,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="47"/>
+      <c r="A192" s="46"/>
       <c r="B192" s="16" t="s">
         <v>45</v>
       </c>
@@ -6452,7 +6488,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="47"/>
+      <c r="A193" s="46"/>
       <c r="B193" s="16" t="s">
         <v>362</v>
       </c>
@@ -6462,7 +6498,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="47"/>
+      <c r="A194" s="46"/>
       <c r="B194" s="16" t="s">
         <v>364</v>
       </c>
@@ -6472,7 +6508,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="47"/>
+      <c r="A195" s="46"/>
       <c r="B195" s="16" t="s">
         <v>366</v>
       </c>
@@ -6482,7 +6518,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="47"/>
+      <c r="A196" s="46"/>
       <c r="B196" s="16" t="s">
         <v>368</v>
       </c>
@@ -6492,7 +6528,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="47"/>
+      <c r="A197" s="46"/>
       <c r="B197" s="16" t="s">
         <v>370</v>
       </c>
@@ -6502,7 +6538,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="47"/>
+      <c r="A198" s="46"/>
       <c r="B198" s="16" t="s">
         <v>372</v>
       </c>
@@ -6512,7 +6548,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="47"/>
+      <c r="A199" s="46"/>
       <c r="B199" s="16" t="s">
         <v>374</v>
       </c>
@@ -6522,7 +6558,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="47"/>
+      <c r="A200" s="46"/>
       <c r="B200" s="16" t="s">
         <v>376</v>
       </c>
@@ -6532,7 +6568,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="47"/>
+      <c r="A201" s="46"/>
       <c r="B201" s="16" t="s">
         <v>378</v>
       </c>
@@ -6542,7 +6578,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="47"/>
+      <c r="A202" s="46"/>
       <c r="B202" s="16" t="s">
         <v>380</v>
       </c>
@@ -6552,7 +6588,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="47"/>
+      <c r="A203" s="46"/>
       <c r="B203" s="16" t="s">
         <v>49</v>
       </c>
@@ -6562,7 +6598,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="47"/>
+      <c r="A204" s="46"/>
       <c r="B204" s="16" t="s">
         <v>383</v>
       </c>
@@ -6572,7 +6608,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="47"/>
+      <c r="A205" s="46"/>
       <c r="B205" s="16" t="s">
         <v>385</v>
       </c>
@@ -6582,7 +6618,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="47"/>
+      <c r="A206" s="46"/>
       <c r="B206" s="16" t="s">
         <v>387</v>
       </c>
@@ -6592,7 +6628,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="47"/>
+      <c r="A207" s="46"/>
       <c r="B207" s="16" t="s">
         <v>389</v>
       </c>
@@ -6602,7 +6638,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="47"/>
+      <c r="A208" s="46"/>
       <c r="B208" s="16" t="s">
         <v>391</v>
       </c>
@@ -6612,7 +6648,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="48"/>
+      <c r="A209" s="47"/>
       <c r="B209" s="18" t="s">
         <v>393</v>
       </c>
@@ -6622,7 +6658,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="49" t="s">
+      <c r="A210" s="48" t="s">
         <v>564</v>
       </c>
       <c r="B210" s="4" t="s">
@@ -6634,7 +6670,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="50"/>
+      <c r="A211" s="49"/>
       <c r="B211" s="5" t="s">
         <v>397</v>
       </c>
@@ -6644,7 +6680,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="50"/>
+      <c r="A212" s="49"/>
       <c r="B212" s="5" t="s">
         <v>399</v>
       </c>
@@ -6654,7 +6690,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="50"/>
+      <c r="A213" s="49"/>
       <c r="B213" s="5" t="s">
         <v>401</v>
       </c>
@@ -6664,7 +6700,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="50"/>
+      <c r="A214" s="49"/>
       <c r="B214" s="5" t="s">
         <v>403</v>
       </c>
@@ -6674,7 +6710,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="50"/>
+      <c r="A215" s="49"/>
       <c r="B215" s="5" t="s">
         <v>405</v>
       </c>
@@ -6684,7 +6720,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="50"/>
+      <c r="A216" s="49"/>
       <c r="B216" s="5" t="s">
         <v>407</v>
       </c>
@@ -6694,7 +6730,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="50"/>
+      <c r="A217" s="49"/>
       <c r="B217" s="5" t="s">
         <v>409</v>
       </c>
@@ -6704,7 +6740,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="50"/>
+      <c r="A218" s="49"/>
       <c r="B218" s="5" t="s">
         <v>411</v>
       </c>
@@ -6714,7 +6750,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="50"/>
+      <c r="A219" s="49"/>
       <c r="B219" s="5" t="s">
         <v>413</v>
       </c>
@@ -6724,7 +6760,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="50"/>
+      <c r="A220" s="49"/>
       <c r="B220" s="5" t="s">
         <v>415</v>
       </c>
@@ -6734,7 +6770,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="50"/>
+      <c r="A221" s="49"/>
       <c r="B221" s="5" t="s">
         <v>417</v>
       </c>
@@ -6744,7 +6780,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="50"/>
+      <c r="A222" s="49"/>
       <c r="B222" s="5" t="s">
         <v>419</v>
       </c>
@@ -6754,7 +6790,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="50"/>
+      <c r="A223" s="49"/>
       <c r="B223" s="5" t="s">
         <v>421</v>
       </c>
@@ -6764,7 +6800,7 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="50"/>
+      <c r="A224" s="49"/>
       <c r="B224" s="5" t="s">
         <v>423</v>
       </c>
@@ -6774,7 +6810,7 @@
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="50"/>
+      <c r="A225" s="49"/>
       <c r="B225" s="5" t="s">
         <v>425</v>
       </c>
@@ -6784,7 +6820,7 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="50"/>
+      <c r="A226" s="49"/>
       <c r="B226" s="5" t="s">
         <v>427</v>
       </c>
@@ -6794,7 +6830,7 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="50"/>
+      <c r="A227" s="49"/>
       <c r="B227" s="5" t="s">
         <v>429</v>
       </c>
@@ -6804,7 +6840,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="50"/>
+      <c r="A228" s="49"/>
       <c r="B228" s="5" t="s">
         <v>431</v>
       </c>
@@ -6814,7 +6850,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="50"/>
+      <c r="A229" s="49"/>
       <c r="B229" s="5" t="s">
         <v>433</v>
       </c>
@@ -6824,7 +6860,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="50"/>
+      <c r="A230" s="49"/>
       <c r="B230" s="5" t="s">
         <v>435</v>
       </c>
@@ -6834,7 +6870,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="50"/>
+      <c r="A231" s="49"/>
       <c r="B231" s="5" t="s">
         <v>437</v>
       </c>
@@ -6844,7 +6880,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="50"/>
+      <c r="A232" s="49"/>
       <c r="B232" s="5" t="s">
         <v>439</v>
       </c>
@@ -6854,7 +6890,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="50"/>
+      <c r="A233" s="49"/>
       <c r="B233" s="5" t="s">
         <v>441</v>
       </c>
@@ -6864,7 +6900,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="50"/>
+      <c r="A234" s="49"/>
       <c r="B234" s="5" t="s">
         <v>443</v>
       </c>
@@ -6874,7 +6910,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="50"/>
+      <c r="A235" s="49"/>
       <c r="B235" s="5" t="s">
         <v>445</v>
       </c>
@@ -6884,7 +6920,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="50"/>
+      <c r="A236" s="49"/>
       <c r="B236" s="5" t="s">
         <v>447</v>
       </c>
@@ -6894,7 +6930,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="50"/>
+      <c r="A237" s="49"/>
       <c r="B237" s="5" t="s">
         <v>449</v>
       </c>
@@ -6904,7 +6940,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="50"/>
+      <c r="A238" s="49"/>
       <c r="B238" s="5" t="s">
         <v>451</v>
       </c>
@@ -6914,7 +6950,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="50"/>
+      <c r="A239" s="49"/>
       <c r="B239" s="5" t="s">
         <v>453</v>
       </c>
@@ -6924,7 +6960,7 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="50"/>
+      <c r="A240" s="49"/>
       <c r="B240" s="5" t="s">
         <v>455</v>
       </c>
@@ -6934,7 +6970,7 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="50"/>
+      <c r="A241" s="49"/>
       <c r="B241" s="5" t="s">
         <v>457</v>
       </c>
@@ -6944,7 +6980,7 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="50"/>
+      <c r="A242" s="49"/>
       <c r="B242" s="5" t="s">
         <v>459</v>
       </c>
@@ -6954,7 +6990,7 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="50"/>
+      <c r="A243" s="49"/>
       <c r="B243" s="5" t="s">
         <v>461</v>
       </c>
@@ -6964,7 +7000,7 @@
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="50"/>
+      <c r="A244" s="49"/>
       <c r="B244" s="5" t="s">
         <v>463</v>
       </c>
@@ -6974,7 +7010,7 @@
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="50"/>
+      <c r="A245" s="49"/>
       <c r="B245" s="5" t="s">
         <v>465</v>
       </c>
@@ -6984,7 +7020,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="50"/>
+      <c r="A246" s="49"/>
       <c r="B246" s="5" t="s">
         <v>467</v>
       </c>
@@ -6994,7 +7030,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="50"/>
+      <c r="A247" s="49"/>
       <c r="B247" s="5" t="s">
         <v>469</v>
       </c>
@@ -7004,7 +7040,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="50"/>
+      <c r="A248" s="49"/>
       <c r="B248" s="5" t="s">
         <v>471</v>
       </c>
@@ -7014,7 +7050,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="50"/>
+      <c r="A249" s="49"/>
       <c r="B249" s="5" t="s">
         <v>473</v>
       </c>
@@ -7024,7 +7060,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="50"/>
+      <c r="A250" s="49"/>
       <c r="B250" s="5" t="s">
         <v>475</v>
       </c>
@@ -7034,7 +7070,7 @@
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="50"/>
+      <c r="A251" s="49"/>
       <c r="B251" s="5" t="s">
         <v>477</v>
       </c>
@@ -7044,7 +7080,7 @@
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="50"/>
+      <c r="A252" s="49"/>
       <c r="B252" s="5" t="s">
         <v>479</v>
       </c>
@@ -7054,7 +7090,7 @@
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="50"/>
+      <c r="A253" s="49"/>
       <c r="B253" s="5" t="s">
         <v>481</v>
       </c>
@@ -7064,7 +7100,7 @@
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="50"/>
+      <c r="A254" s="49"/>
       <c r="B254" s="5" t="s">
         <v>483</v>
       </c>
@@ -7074,7 +7110,7 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="50"/>
+      <c r="A255" s="49"/>
       <c r="B255" s="5" t="s">
         <v>485</v>
       </c>
@@ -7084,7 +7120,7 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="50"/>
+      <c r="A256" s="49"/>
       <c r="B256" s="5" t="s">
         <v>487</v>
       </c>
@@ -7094,7 +7130,7 @@
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="50"/>
+      <c r="A257" s="49"/>
       <c r="B257" s="5" t="s">
         <v>489</v>
       </c>
@@ -7104,7 +7140,7 @@
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A258" s="50"/>
+      <c r="A258" s="49"/>
       <c r="B258" s="5" t="s">
         <v>491</v>
       </c>
@@ -7114,7 +7150,7 @@
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A259" s="50"/>
+      <c r="A259" s="49"/>
       <c r="B259" s="5" t="s">
         <v>493</v>
       </c>
@@ -7124,7 +7160,7 @@
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" s="50"/>
+      <c r="A260" s="49"/>
       <c r="B260" s="5" t="s">
         <v>495</v>
       </c>
@@ -7134,7 +7170,7 @@
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A261" s="50"/>
+      <c r="A261" s="49"/>
       <c r="B261" s="5" t="s">
         <v>497</v>
       </c>
@@ -7144,7 +7180,7 @@
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A262" s="50"/>
+      <c r="A262" s="49"/>
       <c r="B262" s="5" t="s">
         <v>499</v>
       </c>
@@ -7154,7 +7190,7 @@
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A263" s="50"/>
+      <c r="A263" s="49"/>
       <c r="B263" s="5" t="s">
         <v>501</v>
       </c>
@@ -7164,7 +7200,7 @@
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="50"/>
+      <c r="A264" s="49"/>
       <c r="B264" s="5" t="s">
         <v>503</v>
       </c>
@@ -7174,7 +7210,7 @@
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="50"/>
+      <c r="A265" s="49"/>
       <c r="B265" s="5" t="s">
         <v>505</v>
       </c>
@@ -7184,7 +7220,7 @@
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" s="50"/>
+      <c r="A266" s="49"/>
       <c r="B266" s="5" t="s">
         <v>507</v>
       </c>
@@ -7194,7 +7230,7 @@
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="50"/>
+      <c r="A267" s="49"/>
       <c r="B267" s="5" t="s">
         <v>509</v>
       </c>
@@ -7204,7 +7240,7 @@
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" s="50"/>
+      <c r="A268" s="49"/>
       <c r="B268" s="5" t="s">
         <v>511</v>
       </c>
@@ -7214,7 +7250,7 @@
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" s="50"/>
+      <c r="A269" s="49"/>
       <c r="B269" s="5" t="s">
         <v>513</v>
       </c>
@@ -7224,7 +7260,7 @@
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A270" s="50"/>
+      <c r="A270" s="49"/>
       <c r="B270" s="5" t="s">
         <v>515</v>
       </c>
@@ -7234,7 +7270,7 @@
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="50"/>
+      <c r="A271" s="49"/>
       <c r="B271" s="5" t="s">
         <v>517</v>
       </c>
@@ -7244,7 +7280,7 @@
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A272" s="50"/>
+      <c r="A272" s="49"/>
       <c r="B272" s="5" t="s">
         <v>519</v>
       </c>
@@ -7254,7 +7290,7 @@
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="50"/>
+      <c r="A273" s="49"/>
       <c r="B273" s="5" t="s">
         <v>521</v>
       </c>
@@ -7264,7 +7300,7 @@
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="50"/>
+      <c r="A274" s="49"/>
       <c r="B274" s="5" t="s">
         <v>523</v>
       </c>
@@ -7274,7 +7310,7 @@
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="50"/>
+      <c r="A275" s="49"/>
       <c r="B275" s="5" t="s">
         <v>525</v>
       </c>
@@ -7284,7 +7320,7 @@
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A276" s="50"/>
+      <c r="A276" s="49"/>
       <c r="B276" s="5" t="s">
         <v>527</v>
       </c>
@@ -7294,7 +7330,7 @@
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A277" s="50"/>
+      <c r="A277" s="49"/>
       <c r="B277" s="5" t="s">
         <v>529</v>
       </c>
@@ -7304,7 +7340,7 @@
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" s="50"/>
+      <c r="A278" s="49"/>
       <c r="B278" s="5" t="s">
         <v>531</v>
       </c>
@@ -7314,7 +7350,7 @@
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="50"/>
+      <c r="A279" s="49"/>
       <c r="B279" s="5" t="s">
         <v>533</v>
       </c>
@@ -7324,7 +7360,7 @@
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" s="50"/>
+      <c r="A280" s="49"/>
       <c r="B280" s="5" t="s">
         <v>535</v>
       </c>
@@ -7334,7 +7370,7 @@
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="50"/>
+      <c r="A281" s="49"/>
       <c r="B281" s="5" t="s">
         <v>537</v>
       </c>
@@ -7344,7 +7380,7 @@
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" s="50"/>
+      <c r="A282" s="49"/>
       <c r="B282" s="5" t="s">
         <v>539</v>
       </c>
@@ -7354,7 +7390,7 @@
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="50"/>
+      <c r="A283" s="49"/>
       <c r="B283" s="5" t="s">
         <v>541</v>
       </c>
@@ -7364,7 +7400,7 @@
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A284" s="50"/>
+      <c r="A284" s="49"/>
       <c r="B284" s="5" t="s">
         <v>543</v>
       </c>
@@ -7374,7 +7410,7 @@
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A285" s="50"/>
+      <c r="A285" s="49"/>
       <c r="B285" s="5" t="s">
         <v>545</v>
       </c>
@@ -7384,7 +7420,7 @@
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A286" s="50"/>
+      <c r="A286" s="49"/>
       <c r="B286" s="5" t="s">
         <v>547</v>
       </c>
@@ -7394,7 +7430,7 @@
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A287" s="50"/>
+      <c r="A287" s="49"/>
       <c r="B287" s="5" t="s">
         <v>549</v>
       </c>
@@ -7404,7 +7440,7 @@
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A288" s="50"/>
+      <c r="A288" s="49"/>
       <c r="B288" s="5" t="s">
         <v>551</v>
       </c>
@@ -7414,7 +7450,7 @@
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A289" s="50"/>
+      <c r="A289" s="49"/>
       <c r="B289" s="5" t="s">
         <v>553</v>
       </c>
@@ -7424,7 +7460,7 @@
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="50"/>
+      <c r="A290" s="49"/>
       <c r="B290" s="5" t="s">
         <v>555</v>
       </c>
@@ -7434,7 +7470,7 @@
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A291" s="50"/>
+      <c r="A291" s="49"/>
       <c r="B291" s="5" t="s">
         <v>557</v>
       </c>
@@ -7444,7 +7480,7 @@
       </c>
     </row>
     <row r="292" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="51"/>
+      <c r="A292" s="50"/>
       <c r="B292" s="9" t="s">
         <v>559</v>
       </c>
@@ -7454,7 +7490,7 @@
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A293" s="52" t="s">
+      <c r="A293" s="51" t="s">
         <v>565</v>
       </c>
       <c r="B293" s="4" t="s">
@@ -7466,7 +7502,7 @@
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A294" s="53"/>
+      <c r="A294" s="52"/>
       <c r="B294" s="5" t="s">
         <v>188</v>
       </c>
@@ -7476,7 +7512,7 @@
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A295" s="53"/>
+      <c r="A295" s="52"/>
       <c r="B295" s="5" t="s">
         <v>192</v>
       </c>
@@ -7486,7 +7522,7 @@
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A296" s="53"/>
+      <c r="A296" s="52"/>
       <c r="B296" s="5" t="s">
         <v>194</v>
       </c>
@@ -7496,7 +7532,7 @@
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A297" s="53"/>
+      <c r="A297" s="52"/>
       <c r="B297" s="5" t="s">
         <v>196</v>
       </c>
@@ -7506,7 +7542,7 @@
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A298" s="53"/>
+      <c r="A298" s="52"/>
       <c r="B298" s="5" t="s">
         <v>202</v>
       </c>
@@ -7516,7 +7552,7 @@
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A299" s="53"/>
+      <c r="A299" s="52"/>
       <c r="B299" s="5" t="s">
         <v>206</v>
       </c>
@@ -7526,7 +7562,7 @@
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A300" s="53"/>
+      <c r="A300" s="52"/>
       <c r="B300" s="5" t="s">
         <v>209</v>
       </c>
@@ -7536,7 +7572,7 @@
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A301" s="53"/>
+      <c r="A301" s="52"/>
       <c r="B301" s="5" t="s">
         <v>211</v>
       </c>
@@ -7546,7 +7582,7 @@
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A302" s="53"/>
+      <c r="A302" s="52"/>
       <c r="B302" s="5" t="s">
         <v>217</v>
       </c>
@@ -7556,7 +7592,7 @@
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A303" s="53"/>
+      <c r="A303" s="52"/>
       <c r="B303" s="5" t="s">
         <v>223</v>
       </c>
@@ -7566,7 +7602,7 @@
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A304" s="53"/>
+      <c r="A304" s="52"/>
       <c r="B304" s="5" t="s">
         <v>226</v>
       </c>
@@ -7576,7 +7612,7 @@
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A305" s="53"/>
+      <c r="A305" s="52"/>
       <c r="B305" s="5" t="s">
         <v>228</v>
       </c>
@@ -7586,7 +7622,7 @@
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A306" s="53"/>
+      <c r="A306" s="52"/>
       <c r="B306" s="5" t="s">
         <v>230</v>
       </c>
@@ -7596,7 +7632,7 @@
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A307" s="53"/>
+      <c r="A307" s="52"/>
       <c r="B307" s="5" t="s">
         <v>234</v>
       </c>
@@ -7606,7 +7642,7 @@
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A308" s="53"/>
+      <c r="A308" s="52"/>
       <c r="B308" s="5" t="s">
         <v>237</v>
       </c>
@@ -7616,7 +7652,7 @@
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A309" s="53"/>
+      <c r="A309" s="52"/>
       <c r="B309" s="5" t="s">
         <v>242</v>
       </c>
@@ -7626,7 +7662,7 @@
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A310" s="53"/>
+      <c r="A310" s="52"/>
       <c r="B310" s="5" t="s">
         <v>244</v>
       </c>
@@ -7636,7 +7672,7 @@
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A311" s="53"/>
+      <c r="A311" s="52"/>
       <c r="B311" s="5" t="s">
         <v>247</v>
       </c>
@@ -7646,7 +7682,7 @@
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A312" s="53"/>
+      <c r="A312" s="52"/>
       <c r="B312" s="5" t="s">
         <v>250</v>
       </c>
@@ -7656,7 +7692,7 @@
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A313" s="53"/>
+      <c r="A313" s="52"/>
       <c r="B313" s="5" t="s">
         <v>252</v>
       </c>
@@ -7666,7 +7702,7 @@
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A314" s="53"/>
+      <c r="A314" s="52"/>
       <c r="B314" s="5" t="s">
         <v>258</v>
       </c>
@@ -7676,7 +7712,7 @@
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A315" s="53"/>
+      <c r="A315" s="52"/>
       <c r="B315" s="5" t="s">
         <v>260</v>
       </c>
@@ -7686,7 +7722,7 @@
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A316" s="53"/>
+      <c r="A316" s="52"/>
       <c r="B316" s="5" t="s">
         <v>268</v>
       </c>
@@ -7696,7 +7732,7 @@
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A317" s="53"/>
+      <c r="A317" s="52"/>
       <c r="B317" s="5" t="s">
         <v>271</v>
       </c>
@@ -7706,7 +7742,7 @@
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A318" s="53"/>
+      <c r="A318" s="52"/>
       <c r="B318" s="5" t="s">
         <v>273</v>
       </c>
@@ -7716,7 +7752,7 @@
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A319" s="53"/>
+      <c r="A319" s="52"/>
       <c r="B319" s="5" t="s">
         <v>275</v>
       </c>
@@ -7726,7 +7762,7 @@
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A320" s="53"/>
+      <c r="A320" s="52"/>
       <c r="B320" s="5" t="s">
         <v>277</v>
       </c>
@@ -7736,7 +7772,7 @@
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A321" s="53"/>
+      <c r="A321" s="52"/>
       <c r="B321" s="5" t="s">
         <v>279</v>
       </c>
@@ -7746,7 +7782,7 @@
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A322" s="53"/>
+      <c r="A322" s="52"/>
       <c r="B322" s="5" t="s">
         <v>281</v>
       </c>
@@ -7756,7 +7792,7 @@
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A323" s="53"/>
+      <c r="A323" s="52"/>
       <c r="B323" s="5" t="s">
         <v>283</v>
       </c>
@@ -7766,7 +7802,7 @@
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A324" s="53"/>
+      <c r="A324" s="52"/>
       <c r="B324" s="5" t="s">
         <v>289</v>
       </c>
@@ -7776,7 +7812,7 @@
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A325" s="53"/>
+      <c r="A325" s="52"/>
       <c r="B325" s="5" t="s">
         <v>293</v>
       </c>
@@ -7786,7 +7822,7 @@
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A326" s="53"/>
+      <c r="A326" s="52"/>
       <c r="B326" s="5" t="s">
         <v>295</v>
       </c>
@@ -7796,7 +7832,7 @@
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A327" s="53"/>
+      <c r="A327" s="52"/>
       <c r="B327" s="5" t="s">
         <v>297</v>
       </c>
@@ -7806,7 +7842,7 @@
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A328" s="53"/>
+      <c r="A328" s="52"/>
       <c r="B328" s="5" t="s">
         <v>299</v>
       </c>
@@ -7816,7 +7852,7 @@
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A329" s="53"/>
+      <c r="A329" s="52"/>
       <c r="B329" s="5" t="s">
         <v>302</v>
       </c>
@@ -7826,7 +7862,7 @@
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A330" s="53"/>
+      <c r="A330" s="52"/>
       <c r="B330" s="5" t="s">
         <v>304</v>
       </c>
@@ -7836,7 +7872,7 @@
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A331" s="53"/>
+      <c r="A331" s="52"/>
       <c r="B331" s="5" t="s">
         <v>306</v>
       </c>
@@ -7846,7 +7882,7 @@
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A332" s="53"/>
+      <c r="A332" s="52"/>
       <c r="B332" s="5" t="s">
         <v>309</v>
       </c>
@@ -7856,7 +7892,7 @@
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A333" s="53"/>
+      <c r="A333" s="52"/>
       <c r="B333" s="5" t="s">
         <v>313</v>
       </c>
@@ -7866,7 +7902,7 @@
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A334" s="53"/>
+      <c r="A334" s="52"/>
       <c r="B334" s="5" t="s">
         <v>319</v>
       </c>
@@ -7876,7 +7912,7 @@
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A335" s="53"/>
+      <c r="A335" s="52"/>
       <c r="B335" s="5" t="s">
         <v>324</v>
       </c>
@@ -7886,7 +7922,7 @@
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A336" s="53"/>
+      <c r="A336" s="52"/>
       <c r="B336" s="5" t="s">
         <v>326</v>
       </c>
@@ -7896,7 +7932,7 @@
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A337" s="53"/>
+      <c r="A337" s="52"/>
       <c r="B337" s="5" t="s">
         <v>337</v>
       </c>
@@ -7906,7 +7942,7 @@
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A338" s="53"/>
+      <c r="A338" s="52"/>
       <c r="B338" s="5" t="s">
         <v>344</v>
       </c>
@@ -7916,7 +7952,7 @@
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="53"/>
+      <c r="A339" s="52"/>
       <c r="B339" s="5" t="s">
         <v>350</v>
       </c>
@@ -7926,7 +7962,7 @@
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A340" s="53"/>
+      <c r="A340" s="52"/>
       <c r="B340" s="5" t="s">
         <v>352</v>
       </c>
@@ -7936,7 +7972,7 @@
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A341" s="53"/>
+      <c r="A341" s="52"/>
       <c r="B341" s="5" t="s">
         <v>356</v>
       </c>
@@ -7946,7 +7982,7 @@
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A342" s="53"/>
+      <c r="A342" s="52"/>
       <c r="B342" s="5" t="s">
         <v>359</v>
       </c>
@@ -7956,7 +7992,7 @@
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A343" s="53"/>
+      <c r="A343" s="52"/>
       <c r="B343" s="5" t="s">
         <v>364</v>
       </c>
@@ -7966,7 +8002,7 @@
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A344" s="53"/>
+      <c r="A344" s="52"/>
       <c r="B344" s="5" t="s">
         <v>366</v>
       </c>
@@ -7976,7 +8012,7 @@
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A345" s="53"/>
+      <c r="A345" s="52"/>
       <c r="B345" s="5" t="s">
         <v>372</v>
       </c>
@@ -7986,7 +8022,7 @@
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A346" s="53"/>
+      <c r="A346" s="52"/>
       <c r="B346" s="5" t="s">
         <v>374</v>
       </c>
@@ -7996,7 +8032,7 @@
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A347" s="53"/>
+      <c r="A347" s="52"/>
       <c r="B347" s="5" t="s">
         <v>378</v>
       </c>
@@ -8006,7 +8042,7 @@
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A348" s="53"/>
+      <c r="A348" s="52"/>
       <c r="B348" s="5" t="s">
         <v>380</v>
       </c>
@@ -8016,7 +8052,7 @@
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A349" s="53"/>
+      <c r="A349" s="52"/>
       <c r="B349" s="5" t="s">
         <v>383</v>
       </c>
@@ -8026,7 +8062,7 @@
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A350" s="53"/>
+      <c r="A350" s="52"/>
       <c r="B350" s="5" t="s">
         <v>387</v>
       </c>
@@ -8036,7 +8072,7 @@
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A351" s="53"/>
+      <c r="A351" s="52"/>
       <c r="B351" s="5" t="s">
         <v>389</v>
       </c>
@@ -8046,7 +8082,7 @@
       </c>
     </row>
     <row r="352" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A352" s="53"/>
+      <c r="A352" s="52"/>
       <c r="B352" s="9" t="s">
         <v>393</v>
       </c>
@@ -8056,7 +8092,7 @@
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A353" s="43"/>
+      <c r="A353" s="42"/>
       <c r="B353" s="14" t="s">
         <v>565</v>
       </c>
@@ -8068,7 +8104,7 @@
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A354" s="44"/>
+      <c r="A354" s="43"/>
       <c r="B354" s="11" t="s">
         <v>564</v>
       </c>
@@ -8080,7 +8116,7 @@
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A355" s="44"/>
+      <c r="A355" s="43"/>
       <c r="B355" s="11" t="s">
         <v>563</v>
       </c>
@@ -8092,7 +8128,7 @@
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A356" s="44"/>
+      <c r="A356" s="43"/>
       <c r="B356" s="11" t="s">
         <v>176</v>
       </c>
@@ -8104,7 +8140,7 @@
       </c>
     </row>
     <row r="357" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A357" s="45"/>
+      <c r="A357" s="44"/>
       <c r="B357" s="15" t="s">
         <v>562</v>
       </c>
@@ -8133,7 +8169,7 @@
   <dimension ref="B1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>